<commit_message>
Peter-[Update]-create each article analyzer
</commit_message>
<xml_diff>
--- a/analysis_results/ai_analysis/ai_summary.xlsx
+++ b/analysis_results/ai_analysis/ai_summary.xlsx
@@ -10,13 +10,14 @@
     <sheet name="金融產品" sheetId="1" r:id="rId1"/>
     <sheet name="金融機構" sheetId="2" r:id="rId2"/>
     <sheet name="主題分類" sheetId="3" r:id="rId3"/>
+    <sheet name="文章分類" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>產品</t>
   </si>
@@ -24,6 +25,12 @@
     <t>提及次數</t>
   </si>
   <si>
+    <t>信用卡</t>
+  </si>
+  <si>
+    <t>台新@GoGo卡</t>
+  </si>
+  <si>
     <t>信貸專案</t>
   </si>
   <si>
@@ -39,9 +46,6 @@
     <t>數時貸</t>
   </si>
   <si>
-    <t>信用卡</t>
-  </si>
-  <si>
     <t>折扣碼</t>
   </si>
   <si>
@@ -51,42 +55,39 @@
     <t>無線吸塵器</t>
   </si>
   <si>
-    <t>旅行箱</t>
-  </si>
-  <si>
     <t>機構</t>
   </si>
   <si>
     <t>永豐銀行</t>
   </si>
   <si>
+    <t>玉山銀行</t>
+  </si>
+  <si>
+    <t>袋鼠金融</t>
+  </si>
+  <si>
+    <t>台新銀行</t>
+  </si>
+  <si>
+    <t>富邦銀行</t>
+  </si>
+  <si>
+    <t>元富證券</t>
+  </si>
+  <si>
     <t>渣打銀行</t>
   </si>
   <si>
-    <t>富邦信貸</t>
-  </si>
-  <si>
-    <t>遠東商銀</t>
-  </si>
-  <si>
-    <t>玉山銀行</t>
-  </si>
-  <si>
-    <t>KKday</t>
-  </si>
-  <si>
-    <t>袋鼠金融</t>
-  </si>
-  <si>
-    <t>台新銀行</t>
-  </si>
-  <si>
-    <t>中國信託</t>
-  </si>
-  <si>
     <t>滙豐銀行</t>
   </si>
   <si>
+    <t>凱基銀行</t>
+  </si>
+  <si>
+    <t>北富銀行</t>
+  </si>
+  <si>
     <t>主題</t>
   </si>
   <si>
@@ -94,6 +95,60 @@
   </si>
   <si>
     <t>信用卡優惠與稅務相關優惠活動</t>
+  </si>
+  <si>
+    <t>長榮海運的配息政策與股利發放資訊</t>
+  </si>
+  <si>
+    <t>耐吉公司及其股價表現與投資建議</t>
+  </si>
+  <si>
+    <t>王道信貸與國泰信貸的比較及其他信貸方案介紹</t>
+  </si>
+  <si>
+    <t>新戶開戶優惠及投資策略</t>
+  </si>
+  <si>
+    <t>生命靈數的性格特質分析</t>
+  </si>
+  <si>
+    <t>2025年信用卡推薦及權益變動</t>
+  </si>
+  <si>
+    <t>2025年繳稅行事曆及信用卡推薦</t>
+  </si>
+  <si>
+    <t>機場旅平險的保障內容及投保管道比較</t>
+  </si>
+  <si>
+    <t>分類</t>
+  </si>
+  <si>
+    <t>出現次數</t>
+  </si>
+  <si>
+    <t>ROO 投資</t>
+  </si>
+  <si>
+    <t>證券</t>
+  </si>
+  <si>
+    <t>ROO 貸款</t>
+  </si>
+  <si>
+    <t>信貸推薦</t>
+  </si>
+  <si>
+    <t>ROO 時事快訊</t>
+  </si>
+  <si>
+    <t>熱門話題</t>
+  </si>
+  <si>
+    <t>ROO 信用卡</t>
+  </si>
+  <si>
+    <t>信用卡推薦</t>
   </si>
 </sst>
 </file>
@@ -470,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -478,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -571,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -579,7 +634,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -587,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -595,7 +650,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -603,7 +658,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -611,7 +666,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -619,7 +674,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -627,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -635,7 +690,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -643,7 +698,7 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +708,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -674,6 +729,131 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>